<commit_message>
add implementation plan for HRMS
encompassing: start date, length, end date and graph
</commit_message>
<xml_diff>
--- a/PreliminarySchedule.xlsx
+++ b/PreliminarySchedule.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ThaoMy\ITEC\NA\gitHub\need-analysis\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="240" yWindow="60" windowWidth="19440" windowHeight="8010"/>
   </bookViews>
@@ -12,12 +17,12 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
     <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="38">
   <si>
     <t>a</t>
   </si>
@@ -101,6 +106,42 @@
   <si>
     <t>set up enviroment for 
 testing and benchmarking</t>
+  </si>
+  <si>
+    <t>vender selection</t>
+  </si>
+  <si>
+    <t>training users</t>
+  </si>
+  <si>
+    <t>deployment</t>
+  </si>
+  <si>
+    <t>ongoing support</t>
+  </si>
+  <si>
+    <t>detailed discussion</t>
+  </si>
+  <si>
+    <t>implementation planning</t>
+  </si>
+  <si>
+    <t>design the system</t>
+  </si>
+  <si>
+    <t>development the system</t>
+  </si>
+  <si>
+    <t>testing the system</t>
+  </si>
+  <si>
+    <t>modification request</t>
+  </si>
+  <si>
+    <t>create go live plan</t>
+  </si>
+  <si>
+    <t>HRMS project</t>
   </si>
 </sst>
 </file>
@@ -110,7 +151,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-409]d\-mmm\-yyyy;@"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -121,6 +162,14 @@
     <font>
       <b/>
       <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -147,7 +196,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -176,6 +225,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -185,6 +237,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -498,11 +553,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="103724544"/>
-        <c:axId val="103726080"/>
+        <c:axId val="279051208"/>
+        <c:axId val="279055128"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="103724544"/>
+        <c:axId val="279051208"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -525,7 +580,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="103726080"/>
+        <c:crossAx val="279055128"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -533,7 +588,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="103726080"/>
+        <c:axId val="279055128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="42589"/>
@@ -546,7 +601,322 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="103724544"/>
+        <c:crossAx val="279051208"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+        <c:majorUnit val="7"/>
+        <c:minorUnit val="1"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.23030618296788496"/>
+          <c:y val="4.0836395450568677E-2"/>
+          <c:w val="0.7471959143973067"/>
+          <c:h val="0.93323767862350537"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:barChart>
+        <c:barDir val="bar"/>
+        <c:grouping val="stacked"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>start date </c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:noFill/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$20:$A$31</c:f>
+              <c:strCache>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>HRMS project</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>vender selection</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>detailed discussion</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>implementation planning</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>design the system</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>development the system</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>testing the system</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>modification request</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>create go live plan</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>deployment</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>training users</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>ongoing support</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$21:$B$31</c:f>
+              <c:numCache>
+                <c:formatCode>m/d/yyyy</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>42495</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>42501</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>42503</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>42507</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>42516</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>42575</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>42584</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>42593</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>42594</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>42596</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>42598</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>end date</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$20:$A$31</c:f>
+              <c:strCache>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>HRMS project</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>vender selection</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>detailed discussion</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>implementation planning</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>design the system</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>development the system</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>testing the system</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>modification request</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>create go live plan</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>deployment</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>training users</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>ongoing support</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$D$21:$D$31</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>90</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:overlap val="100"/>
+        <c:axId val="98504280"/>
+        <c:axId val="98504672"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="98504280"/>
+        <c:scaling>
+          <c:orientation val="maxMin"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="mm/dd/yy;@" sourceLinked="0"/>
+        <c:majorTickMark val="cross"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="25400"/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="0" vert="horz" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="98504672"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="98504672"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="42690"/>
+          <c:min val="42489"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="t"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="m/d;@" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="98504280"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="7"/>
@@ -569,16 +939,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>28574</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>541324</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>62513</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>247649</xdr:colOff>
-      <xdr:row>62</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>564776</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>62513</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -592,6 +962,38 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>95249</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>5603</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>550127</xdr:colOff>
+      <xdr:row>72</xdr:row>
+      <xdr:rowOff>5603</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -643,7 +1045,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -678,7 +1080,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -889,8 +1291,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E99"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1170,7 +1572,9 @@
       <c r="D19" s="5"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="4"/>
+      <c r="A20" s="12" t="s">
+        <v>37</v>
+      </c>
       <c r="B20" s="6"/>
       <c r="C20" s="9">
         <f t="shared" si="0"/>
@@ -1179,103 +1583,179 @@
       <c r="D20" s="5"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="4"/>
-      <c r="B21" s="6"/>
+      <c r="A21" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B21" s="9">
+        <v>42495</v>
+      </c>
       <c r="C21" s="9">
         <f t="shared" si="0"/>
-        <v>-1</v>
-      </c>
-      <c r="D21" s="5"/>
+        <v>42501</v>
+      </c>
+      <c r="D21" s="5">
+        <v>7</v>
+      </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="4"/>
-      <c r="B22" s="6"/>
+      <c r="A22" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B22" s="9">
+        <f>C21</f>
+        <v>42501</v>
+      </c>
       <c r="C22" s="9">
         <f t="shared" si="0"/>
-        <v>-1</v>
-      </c>
-      <c r="D22" s="5"/>
+        <v>42503</v>
+      </c>
+      <c r="D22" s="5">
+        <v>3</v>
+      </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="4"/>
-      <c r="B23" s="6"/>
+      <c r="A23" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B23" s="6">
+        <f>C22</f>
+        <v>42503</v>
+      </c>
       <c r="C23" s="9">
         <f t="shared" si="0"/>
-        <v>-1</v>
-      </c>
-      <c r="D23" s="5"/>
+        <v>42507</v>
+      </c>
+      <c r="D23" s="5">
+        <v>5</v>
+      </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="4"/>
-      <c r="B24" s="6"/>
+      <c r="A24" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B24" s="6">
+        <f>C23</f>
+        <v>42507</v>
+      </c>
       <c r="C24" s="9">
         <f t="shared" si="0"/>
-        <v>-1</v>
-      </c>
-      <c r="D24" s="5"/>
+        <v>42516</v>
+      </c>
+      <c r="D24" s="5">
+        <v>10</v>
+      </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="4"/>
-      <c r="B25" s="6"/>
+      <c r="A25" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B25" s="6">
+        <f>C24</f>
+        <v>42516</v>
+      </c>
       <c r="C25" s="9">
         <f t="shared" si="0"/>
-        <v>-1</v>
-      </c>
-      <c r="D25" s="5"/>
+        <v>42575</v>
+      </c>
+      <c r="D25" s="5">
+        <v>60</v>
+      </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="4"/>
-      <c r="B26" s="6"/>
+      <c r="A26" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B26" s="6">
+        <f>C25</f>
+        <v>42575</v>
+      </c>
       <c r="C26" s="9">
         <f t="shared" si="0"/>
-        <v>-1</v>
-      </c>
-      <c r="D26" s="5"/>
+        <v>42584</v>
+      </c>
+      <c r="D26" s="5">
+        <v>10</v>
+      </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="4"/>
-      <c r="B27" s="6"/>
+      <c r="A27" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B27" s="6">
+        <f>C26</f>
+        <v>42584</v>
+      </c>
       <c r="C27" s="9">
         <f t="shared" si="0"/>
-        <v>-1</v>
-      </c>
-      <c r="D27" s="5"/>
+        <v>42593</v>
+      </c>
+      <c r="D27" s="5">
+        <v>10</v>
+      </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="4"/>
-      <c r="B28" s="6"/>
+      <c r="A28" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B28" s="6">
+        <f>C27</f>
+        <v>42593</v>
+      </c>
       <c r="C28" s="9">
         <f t="shared" si="0"/>
-        <v>-1</v>
-      </c>
-      <c r="D28" s="5"/>
+        <v>42594</v>
+      </c>
+      <c r="D28" s="5">
+        <v>2</v>
+      </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="4"/>
-      <c r="B29" s="6"/>
+      <c r="A29" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B29" s="6">
+        <f>C28</f>
+        <v>42594</v>
+      </c>
       <c r="C29" s="9">
         <f t="shared" si="0"/>
-        <v>-1</v>
-      </c>
-      <c r="D29" s="5"/>
+        <v>42596</v>
+      </c>
+      <c r="D29" s="5">
+        <v>3</v>
+      </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="4"/>
-      <c r="B30" s="6"/>
+      <c r="A30" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B30" s="6">
+        <f>C29</f>
+        <v>42596</v>
+      </c>
       <c r="C30" s="9">
         <f t="shared" si="0"/>
-        <v>-1</v>
-      </c>
-      <c r="D30" s="5"/>
+        <v>42598</v>
+      </c>
+      <c r="D30" s="5">
+        <v>3</v>
+      </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="4"/>
-      <c r="B31" s="6"/>
+      <c r="A31" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B31" s="6">
+        <f>C30</f>
+        <v>42598</v>
+      </c>
       <c r="C31" s="9">
         <f t="shared" si="0"/>
-        <v>-1</v>
-      </c>
-      <c r="D31" s="5"/>
+        <v>42687</v>
+      </c>
+      <c r="D31" s="5">
+        <v>90</v>
+      </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="4"/>

</xml_diff>